<commit_message>
Added test suite file and updated test method
</commit_message>
<xml_diff>
--- a/datafiles/details.xlsx
+++ b/datafiles/details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\eclipse\selenium-workspace\selenium_project\datafiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF48327C-9DF9-4BCA-B68D-8A8A00F7B08B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4827B013-6372-41C7-BFBE-323CBF117BE6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{B00EF867-E94B-456A-ADE5-F4045A76AC8B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{B00EF867-E94B-456A-ADE5-F4045A76AC8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Valid" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>USERNAME</t>
   </si>
@@ -50,6 +50,12 @@
   </si>
   <si>
     <t>invaliduser</t>
+  </si>
+  <si>
+    <t>ghvg</t>
+  </si>
+  <si>
+    <t>vjhv</t>
   </si>
 </sst>
 </file>
@@ -403,7 +409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6096692-8650-41FD-8193-A96609AD23D1}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -437,8 +443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13D04B35-0FE9-41A6-A2AE-47181FBF9110}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,8 +465,14 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>

</xml_diff>